<commit_message>
Entity and Location update
Added entity and location classes.
</commit_message>
<xml_diff>
--- a/SP4 Proposal and FrameWork/SP4 Gantt Project Planner v1.xlsx
+++ b/SP4 Proposal and FrameWork/SP4 Gantt Project Planner v1.xlsx
@@ -1097,7 +1097,7 @@
   <dimension ref="B2:BQ35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1434,13 +1434,13 @@
         <v>3</v>
       </c>
       <c r="E13" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" s="17">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1517,10 +1517,10 @@
         <v>2</v>
       </c>
       <c r="F17" s="16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="17">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>